<commit_message>
Alteração dos Itens de Configuração
</commit_message>
<xml_diff>
--- a/CSItensConfigv4.xlsx
+++ b/CSItensConfigv4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">Projeto Racha Conta – Conta Share</t>
   </si>
@@ -70,13 +70,31 @@
     <t xml:space="preserve">Diagrama de Classes</t>
   </si>
   <si>
-    <t xml:space="preserve">CSDiaClass v1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caso de Uso</t>
+    <t xml:space="preserve">CSClassD v1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caso de Uso 01</t>
   </si>
   <si>
     <t xml:space="preserve">CSCDU 1 v1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caso de Uso 02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSCDU 2 v1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caso de Uso 03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSCDU 3 v1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caso de Uso 04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSCDU 4 v1.0</t>
   </si>
   <si>
     <t xml:space="preserve">Declaração de Escopo do Projeto</t>
@@ -244,10 +262,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="230" zoomScaleNormal="230" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -328,7 +346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -336,7 +354,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -352,7 +370,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -361,8 +379,32 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>